<commit_message>
Finally got the numbers, next is to build the step of finding if they are active or not
</commit_message>
<xml_diff>
--- a/United_Kingdom_Banks.xlsx
+++ b/United_Kingdom_Banks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks_scrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{2810D760-9CC6-436A-B1C7-91E1A6C6C6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0F2A81F-48C3-4DCD-9998-D71FC11754FE}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{2810D760-9CC6-436A-B1C7-91E1A6C6C6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7695D29C-825B-41A3-99DF-321BEB94B41F}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9C54CCDF-854D-45B7-B0D3-70369417D37B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C54CCDF-854D-45B7-B0D3-70369417D37B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="598">
   <si>
     <t>Name</t>
   </si>
@@ -1414,6 +1414,423 @@
   </si>
   <si>
     <t>1691.57 mln USD</t>
+  </si>
+  <si>
+    <t>Company Number</t>
+  </si>
+  <si>
+    <t>BR014612</t>
+  </si>
+  <si>
+    <t>BR019951</t>
+  </si>
+  <si>
+    <t>NI018800</t>
+  </si>
+  <si>
+    <t>BR018263</t>
+  </si>
+  <si>
+    <t>BR011722</t>
+  </si>
+  <si>
+    <t>BR020302</t>
+  </si>
+  <si>
+    <t>BR000580</t>
+  </si>
+  <si>
+    <t>BR001254</t>
+  </si>
+  <si>
+    <t>BR017492</t>
+  </si>
+  <si>
+    <t>BR018431</t>
+  </si>
+  <si>
+    <t>BR001769</t>
+  </si>
+  <si>
+    <t>BR001085</t>
+  </si>
+  <si>
+    <t>BR000356</t>
+  </si>
+  <si>
+    <t>BR008339</t>
+  </si>
+  <si>
+    <t>BR001358</t>
+  </si>
+  <si>
+    <t>BR002014</t>
+  </si>
+  <si>
+    <t>BR001417</t>
+  </si>
+  <si>
+    <t>BR018625</t>
+  </si>
+  <si>
+    <t>BR001344</t>
+  </si>
+  <si>
+    <t>BR001992</t>
+  </si>
+  <si>
+    <t>BR000521</t>
+  </si>
+  <si>
+    <t>SC327000</t>
+  </si>
+  <si>
+    <t>BR007739</t>
+  </si>
+  <si>
+    <t>BR021986</t>
+  </si>
+  <si>
+    <t>BR014651</t>
+  </si>
+  <si>
+    <t>BR009959</t>
+  </si>
+  <si>
+    <t>BR001571</t>
+  </si>
+  <si>
+    <t>BR000790</t>
+  </si>
+  <si>
+    <t>BR021724</t>
+  </si>
+  <si>
+    <t>BR000170</t>
+  </si>
+  <si>
+    <t>BR000151</t>
+  </si>
+  <si>
+    <t>BR000397</t>
+  </si>
+  <si>
+    <t>BR000783</t>
+  </si>
+  <si>
+    <t>BR000414</t>
+  </si>
+  <si>
+    <t>BR017263</t>
+  </si>
+  <si>
+    <t>BR017382</t>
+  </si>
+  <si>
+    <t>BR013933</t>
+  </si>
+  <si>
+    <t>BR005291</t>
+  </si>
+  <si>
+    <t>BIC </t>
+  </si>
+  <si>
+    <t>BR001018</t>
+  </si>
+  <si>
+    <t>SC001111</t>
+  </si>
+  <si>
+    <t>BR001025</t>
+  </si>
+  <si>
+    <t>BR000250</t>
+  </si>
+  <si>
+    <t>BR002630</t>
+  </si>
+  <si>
+    <t>BR001975</t>
+  </si>
+  <si>
+    <t>BR000705</t>
+  </si>
+  <si>
+    <t>FC007227</t>
+  </si>
+  <si>
+    <t>BR000080</t>
+  </si>
+  <si>
+    <t>BR000664</t>
+  </si>
+  <si>
+    <t>BR000005</t>
+  </si>
+  <si>
+    <t>BR007517</t>
+  </si>
+  <si>
+    <t>BR000001</t>
+  </si>
+  <si>
+    <t>BR009373</t>
+  </si>
+  <si>
+    <t>BR014405</t>
+  </si>
+  <si>
+    <t>BR004789</t>
+  </si>
+  <si>
+    <t>BR017561</t>
+  </si>
+  <si>
+    <t>BR000163</t>
+  </si>
+  <si>
+    <t>BR001616</t>
+  </si>
+  <si>
+    <t>BR010027</t>
+  </si>
+  <si>
+    <t>BR016197</t>
+  </si>
+  <si>
+    <t>BR011218</t>
+  </si>
+  <si>
+    <t>BR000953</t>
+  </si>
+  <si>
+    <t>BR007625</t>
+  </si>
+  <si>
+    <t>BR004735</t>
+  </si>
+  <si>
+    <t>BR016253</t>
+  </si>
+  <si>
+    <t>BR016211</t>
+  </si>
+  <si>
+    <t>BR008908</t>
+  </si>
+  <si>
+    <t>MFI ID </t>
+  </si>
+  <si>
+    <t>BR000036</t>
+  </si>
+  <si>
+    <t>BR020919</t>
+  </si>
+  <si>
+    <t>BR000746</t>
+  </si>
+  <si>
+    <t>BR004567</t>
+  </si>
+  <si>
+    <t>BR010157</t>
+  </si>
+  <si>
+    <t>BR010262</t>
+  </si>
+  <si>
+    <t>BR020187</t>
+  </si>
+  <si>
+    <t>BR000273</t>
+  </si>
+  <si>
+    <t>BR000011</t>
+  </si>
+  <si>
+    <t>BR016782</t>
+  </si>
+  <si>
+    <t>BR002678</t>
+  </si>
+  <si>
+    <t>BR001636</t>
+  </si>
+  <si>
+    <t>BR001223</t>
+  </si>
+  <si>
+    <t>BR009581</t>
+  </si>
+  <si>
+    <t>BR000596</t>
+  </si>
+  <si>
+    <t>BR001446</t>
+  </si>
+  <si>
+    <t>BR002048</t>
+  </si>
+  <si>
+    <t>BR002013</t>
+  </si>
+  <si>
+    <t>BR020674</t>
+  </si>
+  <si>
+    <t>BR001924</t>
+  </si>
+  <si>
+    <t>BR000290</t>
+  </si>
+  <si>
+    <t>BR005650</t>
+  </si>
+  <si>
+    <t>BR001334</t>
+  </si>
+  <si>
+    <t>BR010261</t>
+  </si>
+  <si>
+    <t>BR000306</t>
+  </si>
+  <si>
+    <t>BR017147</t>
+  </si>
+  <si>
+    <t>NI004467</t>
+  </si>
+  <si>
+    <t>BR000981</t>
+  </si>
+  <si>
+    <t>BR005808</t>
+  </si>
+  <si>
+    <t>BR000445</t>
+  </si>
+  <si>
+    <t>BR001982</t>
+  </si>
+  <si>
+    <t>BR014846</t>
+  </si>
+  <si>
+    <t>BR003696</t>
+  </si>
+  <si>
+    <t>BR000548</t>
+  </si>
+  <si>
+    <t>BR001487</t>
+  </si>
+  <si>
+    <t>BR016556</t>
+  </si>
+  <si>
+    <t>BR008721</t>
+  </si>
+  <si>
+    <t>BR000021</t>
+  </si>
+  <si>
+    <t>ZC000018</t>
+  </si>
+  <si>
+    <t>BR000696</t>
+  </si>
+  <si>
+    <t>BR002088</t>
+  </si>
+  <si>
+    <t>BR009903</t>
+  </si>
+  <si>
+    <t>BR007234</t>
+  </si>
+  <si>
+    <t>BR019790</t>
+  </si>
+  <si>
+    <t>BR000732</t>
+  </si>
+  <si>
+    <t>BR001736</t>
+  </si>
+  <si>
+    <t>SC173199</t>
+  </si>
+  <si>
+    <t>BR000818</t>
+  </si>
+  <si>
+    <t>BR014361</t>
+  </si>
+  <si>
+    <t>BR010889</t>
+  </si>
+  <si>
+    <t>BR000798</t>
+  </si>
+  <si>
+    <t>RC000042</t>
+  </si>
+  <si>
+    <t>BR001944</t>
+  </si>
+  <si>
+    <t>BR004065</t>
+  </si>
+  <si>
+    <t>BR001902</t>
+  </si>
+  <si>
+    <t>BR019279</t>
+  </si>
+  <si>
+    <t>SC083026</t>
+  </si>
+  <si>
+    <t>BR001499</t>
+  </si>
+  <si>
+    <t>SC095237</t>
+  </si>
+  <si>
+    <t>BR001619</t>
+  </si>
+  <si>
+    <t>BR004507</t>
+  </si>
+  <si>
+    <t>R0000733</t>
+  </si>
+  <si>
+    <t>BR001757</t>
+  </si>
+  <si>
+    <t>BR001786</t>
+  </si>
+  <si>
+    <t>BR000994</t>
+  </si>
+  <si>
+    <t>BR002012</t>
+  </si>
+  <si>
+    <t>BR009065</t>
+  </si>
+  <si>
+    <t>BR009910</t>
+  </si>
+  <si>
+    <t>BR000106</t>
+  </si>
+  <si>
+    <t>BR001980</t>
   </si>
 </sst>
 </file>
@@ -1765,19 +2182,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0953D09C-EEC6-4C19-A530-793F572717AA}">
-  <dimension ref="A1:D267"/>
+  <dimension ref="A1:E268"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E267" sqref="E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1790,8 +2208,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1804,8 +2225,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2564490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1815,8 +2239,11 @@
       <c r="C3">
         <v>-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1826,8 +2253,11 @@
       <c r="C4">
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1840,8 +2270,11 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1854,8 +2287,11 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4483430</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1868,8 +2304,11 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>947662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1882,8 +2321,11 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>185070</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1893,8 +2335,11 @@
       <c r="C9">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1904,8 +2349,11 @@
       <c r="C10">
         <v>-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1918,8 +2366,11 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1929,8 +2380,11 @@
       <c r="C12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1943,8 +2397,11 @@
       <c r="D13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>8632552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1954,8 +2411,11 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1968,8 +2428,11 @@
       <c r="D15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>7554558</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1979,8 +2442,11 @@
       <c r="C16">
         <v>-3.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1990,8 +2456,11 @@
       <c r="C17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2001,8 +2470,11 @@
       <c r="C18">
         <v>-1.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2012,8 +2484,11 @@
       <c r="C19">
         <v>-1.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2023,8 +2498,11 @@
       <c r="C20">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2034,8 +2512,11 @@
       <c r="C21">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2048,8 +2529,11 @@
       <c r="D22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>980698</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2062,8 +2546,11 @@
       <c r="D23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>640370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2076,8 +2563,11 @@
       <c r="D24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>3793679</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2087,8 +2577,11 @@
       <c r="C25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2098,8 +2591,11 @@
       <c r="C26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2109,8 +2605,11 @@
       <c r="C27">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -2123,8 +2622,11 @@
       <c r="D28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>10826803</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -2137,8 +2639,11 @@
       <c r="D29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>4406777</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2151,8 +2656,11 @@
       <c r="D30" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>6736473</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2165,8 +2673,11 @@
       <c r="D31" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>6193060</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -2176,8 +2687,11 @@
       <c r="C32">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -2187,8 +2701,11 @@
       <c r="C33">
         <v>-2.2999999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -2198,8 +2715,11 @@
       <c r="C34">
         <v>-3.8</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2209,8 +2729,11 @@
       <c r="C35">
         <v>-3.1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2220,8 +2743,11 @@
       <c r="C36">
         <v>-2.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>7022885</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2234,8 +2760,11 @@
       <c r="D37" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>5897786</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -2245,8 +2774,11 @@
       <c r="C38">
         <v>-5</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2259,8 +2791,11 @@
       <c r="D39" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -2270,8 +2805,11 @@
       <c r="C40" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -2284,8 +2822,11 @@
       <c r="D41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>5888535</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -2298,8 +2839,11 @@
       <c r="D42" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>1126618</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -2312,8 +2856,11 @@
       <c r="D43" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>4189598</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -2323,8 +2870,11 @@
       <c r="C44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2334,8 +2884,11 @@
       <c r="C45" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -2345,8 +2898,11 @@
       <c r="C46" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -2359,8 +2915,11 @@
       <c r="D47" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>1026167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -2373,8 +2932,11 @@
       <c r="D48" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>9740322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2384,8 +2946,11 @@
       <c r="C49" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2398,8 +2963,11 @@
       <c r="D50" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>4797759</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -2409,8 +2977,11 @@
       <c r="C51">
         <v>-4.5999999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -2423,8 +2994,11 @@
       <c r="D52" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>5321714</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -2434,8 +3008,11 @@
       <c r="C53" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -2445,8 +3022,11 @@
       <c r="C54">
         <v>-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -2459,8 +3039,11 @@
       <c r="D55" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>1047302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -2473,8 +3056,11 @@
       <c r="D56" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -2484,8 +3070,11 @@
       <c r="C57">
         <v>-5</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -2498,8 +3087,11 @@
       <c r="D58" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2512,8 +3104,11 @@
       <c r="D59" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>1837656</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -2526,8 +3121,11 @@
       <c r="D60" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -2537,8 +3135,11 @@
       <c r="C61">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2548,8 +3149,11 @@
       <c r="C62">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -2562,8 +3166,11 @@
       <c r="D63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>2572704</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -2573,8 +3180,11 @@
       <c r="C64" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>124</v>
       </c>
@@ -2587,8 +3197,11 @@
       <c r="D65" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>9964966</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>126</v>
       </c>
@@ -2598,8 +3211,11 @@
       <c r="C66" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -2612,8 +3228,11 @@
       <c r="D67" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>6455352</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -2623,8 +3242,11 @@
       <c r="C68">
         <v>-5</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>130</v>
       </c>
@@ -2634,8 +3256,11 @@
       <c r="C69">
         <v>-3.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>131</v>
       </c>
@@ -2648,8 +3273,11 @@
       <c r="D70" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>2733036</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -2659,8 +3287,11 @@
       <c r="C71">
         <v>-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -2670,8 +3301,11 @@
       <c r="C72">
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -2681,8 +3315,11 @@
       <c r="C73">
         <v>-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2692,8 +3329,11 @@
       <c r="C74" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>9736376</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2706,8 +3346,11 @@
       <c r="D75" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>195626</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>142</v>
       </c>
@@ -2720,8 +3363,11 @@
       <c r="D76" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>144</v>
       </c>
@@ -2731,8 +3377,11 @@
       <c r="C77" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>145</v>
       </c>
@@ -2742,8 +3391,11 @@
       <c r="C78">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>146</v>
       </c>
@@ -2753,8 +3405,11 @@
       <c r="C79">
         <v>-4.5999999999999996</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2767,8 +3422,11 @@
       <c r="D80" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2778,8 +3436,11 @@
       <c r="C81">
         <v>-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>150</v>
       </c>
@@ -2789,8 +3450,11 @@
       <c r="C82">
         <v>-1.9</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>151</v>
       </c>
@@ -2800,8 +3464,11 @@
       <c r="C83">
         <v>-3.2</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>152</v>
       </c>
@@ -2814,8 +3481,11 @@
       <c r="D84" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>2500199</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>154</v>
       </c>
@@ -2828,8 +3498,11 @@
       <c r="D85" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>2334687</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>156</v>
       </c>
@@ -2842,8 +3515,11 @@
       <c r="D86" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>4728421</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>158</v>
       </c>
@@ -2853,8 +3529,11 @@
       <c r="C87">
         <v>-2.9</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -2864,8 +3543,11 @@
       <c r="C88">
         <v>-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>160</v>
       </c>
@@ -2875,8 +3557,11 @@
       <c r="C89">
         <v>-1.6</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>161</v>
       </c>
@@ -2886,8 +3571,11 @@
       <c r="C90">
         <v>-5</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>162</v>
       </c>
@@ -2897,8 +3585,11 @@
       <c r="C91">
         <v>-5</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>163</v>
       </c>
@@ -2911,8 +3602,11 @@
       <c r="D92" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>2321802</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>166</v>
       </c>
@@ -2922,8 +3616,11 @@
       <c r="C93" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>168</v>
       </c>
@@ -2933,8 +3630,11 @@
       <c r="C94">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -2944,8 +3644,11 @@
       <c r="C95">
         <v>-1</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>170</v>
       </c>
@@ -2955,8 +3658,11 @@
       <c r="C96" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>171</v>
       </c>
@@ -2969,8 +3675,11 @@
       <c r="D97" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>5575857</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>173</v>
       </c>
@@ -2983,8 +3692,11 @@
       <c r="D98" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>4459383</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>175</v>
       </c>
@@ -2997,8 +3709,11 @@
       <c r="D99" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>772784</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>178</v>
       </c>
@@ -3011,8 +3726,11 @@
       <c r="D100" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>6621225</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>180</v>
       </c>
@@ -3025,8 +3743,11 @@
       <c r="D101" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>2856884</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>182</v>
       </c>
@@ -3036,8 +3757,11 @@
       <c r="C102">
         <v>-1.8</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>183</v>
       </c>
@@ -3047,8 +3771,11 @@
       <c r="C103">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>184</v>
       </c>
@@ -3058,8 +3785,11 @@
       <c r="C104">
         <v>-5</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>185</v>
       </c>
@@ -3069,8 +3799,11 @@
       <c r="C105" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>10631597</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>187</v>
       </c>
@@ -3083,8 +3816,11 @@
       <c r="D106" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>3468216</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>190</v>
       </c>
@@ -3094,8 +3830,11 @@
       <c r="C107" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>191</v>
       </c>
@@ -3108,8 +3847,11 @@
       <c r="D108" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>1122503</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>193</v>
       </c>
@@ -3122,8 +3864,11 @@
       <c r="D109" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>5969821</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>195</v>
       </c>
@@ -3133,8 +3878,11 @@
       <c r="C110">
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -3144,8 +3892,11 @@
       <c r="C111">
         <v>-4</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>197</v>
       </c>
@@ -3158,8 +3909,11 @@
       <c r="D112" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <v>8864609</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>199</v>
       </c>
@@ -3172,8 +3926,11 @@
       <c r="D113" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>201</v>
       </c>
@@ -3186,8 +3943,11 @@
       <c r="D114" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <v>1311315</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>204</v>
       </c>
@@ -3200,8 +3960,11 @@
       <c r="D115" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <v>11305395</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>206</v>
       </c>
@@ -3211,8 +3974,11 @@
       <c r="C116" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>207</v>
       </c>
@@ -3225,8 +3991,11 @@
       <c r="D117" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <v>1074897</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>210</v>
       </c>
@@ -3239,8 +4008,11 @@
       <c r="D118" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <v>1719649</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>212</v>
       </c>
@@ -3253,8 +4025,11 @@
       <c r="D119" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>14259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>214</v>
       </c>
@@ -3264,8 +4039,11 @@
       <c r="C120">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>215</v>
       </c>
@@ -3278,8 +4056,11 @@
       <c r="D121" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>499482</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>217</v>
       </c>
@@ -3292,8 +4073,11 @@
       <c r="D122" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <v>9928412</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>219</v>
       </c>
@@ -3303,8 +4087,11 @@
       <c r="C123" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>220</v>
       </c>
@@ -3317,8 +4104,11 @@
       <c r="D124" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124">
+        <v>4552753</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>222</v>
       </c>
@@ -3331,8 +4121,11 @@
       <c r="D125" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>2130447</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>224</v>
       </c>
@@ -3345,8 +4138,11 @@
       <c r="D126" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126">
+        <v>4663024</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>226</v>
       </c>
@@ -3356,8 +4152,11 @@
       <c r="C127">
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>227</v>
       </c>
@@ -3367,8 +4166,11 @@
       <c r="C128">
         <v>-3</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>228</v>
       </c>
@@ -3378,8 +4180,11 @@
       <c r="C129">
         <v>-5</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>229</v>
       </c>
@@ -3389,8 +4194,11 @@
       <c r="C130">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>231</v>
       </c>
@@ -3400,8 +4208,11 @@
       <c r="C131">
         <v>-3.3</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>232</v>
       </c>
@@ -3414,8 +4225,11 @@
       <c r="D132" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132">
+        <v>7425398</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>234</v>
       </c>
@@ -3425,8 +4239,11 @@
       <c r="C133" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>235</v>
       </c>
@@ -3439,8 +4256,11 @@
       <c r="D134" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>938937</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>237</v>
       </c>
@@ -3453,8 +4273,11 @@
       <c r="D135" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135">
+        <v>1814093</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>239</v>
       </c>
@@ -3464,8 +4287,11 @@
       <c r="C136">
         <v>-1.8</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>240</v>
       </c>
@@ -3475,8 +4301,11 @@
       <c r="C137">
         <v>-4</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>241</v>
       </c>
@@ -3486,8 +4315,11 @@
       <c r="C138">
         <v>-5</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>242</v>
       </c>
@@ -3500,8 +4332,11 @@
       <c r="D139" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>2693038</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>244</v>
       </c>
@@ -3511,8 +4346,11 @@
       <c r="C140" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>245</v>
       </c>
@@ -3525,8 +4363,11 @@
       <c r="D141" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>4346834</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>248</v>
       </c>
@@ -3536,8 +4377,11 @@
       <c r="C142" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -3547,8 +4391,11 @@
       <c r="C143">
         <v>-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>250</v>
       </c>
@@ -3558,8 +4405,11 @@
       <c r="C144">
         <v>-5</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>251</v>
       </c>
@@ -3572,8 +4422,11 @@
       <c r="D145" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145">
+        <v>10399850</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>253</v>
       </c>
@@ -3586,8 +4439,11 @@
       <c r="D146" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>255</v>
       </c>
@@ -3597,8 +4453,11 @@
       <c r="C147">
         <v>-5</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>256</v>
       </c>
@@ -3611,8 +4470,11 @@
       <c r="D148" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148">
+        <v>6309906</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>259</v>
       </c>
@@ -3622,8 +4484,11 @@
       <c r="C149">
         <v>-4</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>260</v>
       </c>
@@ -3636,8 +4501,11 @@
       <c r="D150" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150">
+        <v>3704031</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>262</v>
       </c>
@@ -3647,8 +4515,11 @@
       <c r="C151">
         <v>-4.5999999999999996</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>263</v>
       </c>
@@ -3661,8 +4532,11 @@
       <c r="D152" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>265</v>
       </c>
@@ -3672,8 +4546,11 @@
       <c r="C153">
         <v>-5</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>266</v>
       </c>
@@ -3686,8 +4563,11 @@
       <c r="D154" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154">
+        <v>9660012</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>268</v>
       </c>
@@ -3697,8 +4577,11 @@
       <c r="C155">
         <v>-5</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>269</v>
       </c>
@@ -3711,8 +4594,11 @@
       <c r="D156" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>4152338</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>271</v>
       </c>
@@ -3725,8 +4611,11 @@
       <c r="D157" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157">
+        <v>30546</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>273</v>
       </c>
@@ -3739,8 +4628,11 @@
       <c r="D158" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158">
+        <v>6419578</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>275</v>
       </c>
@@ -3750,8 +4642,11 @@
       <c r="C159">
         <v>-5</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>277</v>
       </c>
@@ -3761,8 +4656,11 @@
       <c r="C160">
         <v>-5</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>279</v>
       </c>
@@ -3772,8 +4670,11 @@
       <c r="C161">
         <v>-4.4000000000000004</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>280</v>
       </c>
@@ -3786,8 +4687,11 @@
       <c r="D162" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162">
+        <v>1203696</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>282</v>
       </c>
@@ -3797,8 +4701,11 @@
       <c r="C163" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163">
+        <v>10921940</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>283</v>
       </c>
@@ -3811,8 +4718,11 @@
       <c r="D164" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164">
+        <v>9446231</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>285</v>
       </c>
@@ -3825,8 +4735,11 @@
       <c r="D165" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165">
+        <v>2068222</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>288</v>
       </c>
@@ -3836,8 +4749,11 @@
       <c r="C166">
         <v>-5</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>289</v>
       </c>
@@ -3847,8 +4763,11 @@
       <c r="C167" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>290</v>
       </c>
@@ -3858,8 +4777,11 @@
       <c r="C168" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>291</v>
       </c>
@@ -3872,8 +4794,11 @@
       <c r="D169" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169">
+        <v>2743734</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>293</v>
       </c>
@@ -3883,8 +4808,11 @@
       <c r="C170">
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>294</v>
       </c>
@@ -3897,8 +4825,11 @@
       <c r="D171" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171">
+        <v>2773743</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>296</v>
       </c>
@@ -3911,8 +4842,11 @@
       <c r="D172" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172">
+        <v>929027</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>298</v>
       </c>
@@ -3922,8 +4856,11 @@
       <c r="C173">
         <v>-1.3</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>299</v>
       </c>
@@ -3933,8 +4870,11 @@
       <c r="C174">
         <v>-2</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>300</v>
       </c>
@@ -3944,8 +4884,11 @@
       <c r="C175">
         <v>-2.2999999999999998</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>301</v>
       </c>
@@ -3958,8 +4901,11 @@
       <c r="D176" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176">
+        <v>1981122</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>303</v>
       </c>
@@ -3969,8 +4915,11 @@
       <c r="C177">
         <v>-5</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>304</v>
       </c>
@@ -3980,8 +4929,11 @@
       <c r="C178">
         <v>-3.5</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>305</v>
       </c>
@@ -3994,8 +4946,11 @@
       <c r="D179" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>308</v>
       </c>
@@ -4005,8 +4960,11 @@
       <c r="C180" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>309</v>
       </c>
@@ -4019,8 +4977,11 @@
       <c r="D181" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181">
+        <v>5390593</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>311</v>
       </c>
@@ -4033,8 +4994,11 @@
       <c r="D182" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182">
+        <v>2794633</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>313</v>
       </c>
@@ -4047,8 +5011,11 @@
       <c r="D183" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183">
+        <v>4218020</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>315</v>
       </c>
@@ -4061,8 +5028,11 @@
       <c r="D184" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184">
+        <v>2939223</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>317</v>
       </c>
@@ -4072,8 +5042,11 @@
       <c r="C185" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>318</v>
       </c>
@@ -4083,8 +5056,11 @@
       <c r="C186">
         <v>-3.6</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>319</v>
       </c>
@@ -4097,8 +5073,11 @@
       <c r="D187" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187">
+        <v>5781326</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>321</v>
       </c>
@@ -4108,8 +5087,11 @@
       <c r="C188">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>322</v>
       </c>
@@ -4122,8 +5104,11 @@
       <c r="D189" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189">
+        <v>4656003</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>325</v>
       </c>
@@ -4136,8 +5121,11 @@
       <c r="D190" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>327</v>
       </c>
@@ -4147,8 +5135,11 @@
       <c r="C191">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>328</v>
       </c>
@@ -4161,8 +5152,11 @@
       <c r="D192" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192">
+        <v>995939</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>330</v>
       </c>
@@ -4172,8 +5166,11 @@
       <c r="C193">
         <v>-2.4</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E193">
+        <v>11429127</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>331</v>
       </c>
@@ -4186,8 +5183,11 @@
       <c r="D194" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E194">
+        <v>9872265</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>334</v>
       </c>
@@ -4200,8 +5200,11 @@
       <c r="D195" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E195">
+        <v>68835</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>336</v>
       </c>
@@ -4211,8 +5214,11 @@
       <c r="C196">
         <v>-3.3</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>338</v>
       </c>
@@ -4222,8 +5228,11 @@
       <c r="C197">
         <v>-4</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E197" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>339</v>
       </c>
@@ -4236,8 +5245,11 @@
       <c r="D198" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>341</v>
       </c>
@@ -4250,8 +5262,11 @@
       <c r="D199" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199">
+        <v>2338548</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>343</v>
       </c>
@@ -4264,8 +5279,11 @@
       <c r="D200" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200">
+        <v>2294747</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>345</v>
       </c>
@@ -4278,8 +5296,11 @@
       <c r="D201" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201">
+        <v>817692</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>347</v>
       </c>
@@ -4292,8 +5313,11 @@
       <c r="D202" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202">
+        <v>541132</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>349</v>
       </c>
@@ -4306,8 +5330,11 @@
       <c r="D203" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203">
+        <v>964058</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>351</v>
       </c>
@@ -4317,8 +5344,11 @@
       <c r="C204">
         <v>-4.7</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>352</v>
       </c>
@@ -4328,8 +5358,11 @@
       <c r="C205" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>353</v>
       </c>
@@ -4342,8 +5375,11 @@
       <c r="D206" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206">
+        <v>388466</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>355</v>
       </c>
@@ -4353,8 +5389,11 @@
       <c r="C207">
         <v>-5</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>356</v>
       </c>
@@ -4364,8 +5403,11 @@
       <c r="C208">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -4375,8 +5417,11 @@
       <c r="C209" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209">
+        <v>4684034</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>358</v>
       </c>
@@ -4386,8 +5431,11 @@
       <c r="C210">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>359</v>
       </c>
@@ -4400,8 +5448,11 @@
       <c r="D211" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211">
+        <v>3792250</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -4414,8 +5465,11 @@
       <c r="D212" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>364</v>
       </c>
@@ -4428,8 +5482,11 @@
       <c r="D213" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213">
+        <v>9092149</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>366</v>
       </c>
@@ -4439,8 +5496,11 @@
       <c r="C214">
         <v>-2.8</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>367</v>
       </c>
@@ -4450,8 +5510,11 @@
       <c r="C215" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>368</v>
       </c>
@@ -4461,8 +5524,11 @@
       <c r="C216">
         <v>-3.8</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>369</v>
       </c>
@@ -4472,8 +5538,11 @@
       <c r="C217" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>370</v>
       </c>
@@ -4483,8 +5552,11 @@
       <c r="C218" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>371</v>
       </c>
@@ -4494,8 +5566,11 @@
       <c r="C219">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>372</v>
       </c>
@@ -4505,8 +5580,11 @@
       <c r="C220">
         <v>-4.2</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>373</v>
       </c>
@@ -4519,8 +5597,11 @@
       <c r="D221" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221">
+        <v>955491</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>375</v>
       </c>
@@ -4533,8 +5614,11 @@
       <c r="D222" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222">
+        <v>2734652</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>377</v>
       </c>
@@ -4547,8 +5631,11 @@
       <c r="D223" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>379</v>
       </c>
@@ -4561,8 +5648,11 @@
       <c r="D224" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224">
+        <v>6365062</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>382</v>
       </c>
@@ -4572,8 +5662,11 @@
       <c r="C225" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>383</v>
       </c>
@@ -4586,8 +5679,11 @@
       <c r="D226" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226">
+        <v>3236121</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>385</v>
       </c>
@@ -4597,8 +5693,11 @@
       <c r="C227" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>386</v>
       </c>
@@ -4608,8 +5707,11 @@
       <c r="C228">
         <v>-1.5</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>387</v>
       </c>
@@ -4622,8 +5724,11 @@
       <c r="D229" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229">
+        <v>4330018</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>390</v>
       </c>
@@ -4633,8 +5738,11 @@
       <c r="C230" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>391</v>
       </c>
@@ -4647,8 +5755,11 @@
       <c r="D231" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231">
+        <v>990937</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>393</v>
       </c>
@@ -4658,8 +5769,11 @@
       <c r="C232">
         <v>-3.9</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>395</v>
       </c>
@@ -4669,8 +5783,11 @@
       <c r="C233">
         <v>-1.5</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>396</v>
       </c>
@@ -4680,8 +5797,11 @@
       <c r="C234">
         <v>-2.1</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>397</v>
       </c>
@@ -4691,8 +5811,11 @@
       <c r="C235" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>398</v>
       </c>
@@ -4702,8 +5825,11 @@
       <c r="C236">
         <v>-5</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>400</v>
       </c>
@@ -4713,8 +5839,11 @@
       <c r="C237">
         <v>-3</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>402</v>
       </c>
@@ -4727,8 +5856,11 @@
       <c r="D238" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>404</v>
       </c>
@@ -4738,8 +5870,11 @@
       <c r="C239">
         <v>-4</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>405</v>
       </c>
@@ -4752,8 +5887,11 @@
       <c r="D240" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240">
+        <v>11379025</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>408</v>
       </c>
@@ -4766,8 +5904,11 @@
       <c r="D241" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>410</v>
       </c>
@@ -4780,8 +5921,11 @@
       <c r="D242" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242">
+        <v>2643004</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>412</v>
       </c>
@@ -4791,8 +5935,11 @@
       <c r="C243">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E243" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>413</v>
       </c>
@@ -4802,8 +5949,11 @@
       <c r="C244">
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>414</v>
       </c>
@@ -4816,8 +5966,11 @@
       <c r="D245" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>416</v>
       </c>
@@ -4827,8 +5980,11 @@
       <c r="C246">
         <v>-3.3</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>417</v>
       </c>
@@ -4838,8 +5994,11 @@
       <c r="C247">
         <v>-3.3</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>418</v>
       </c>
@@ -4849,8 +6008,11 @@
       <c r="C248">
         <v>-5</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>420</v>
       </c>
@@ -4863,8 +6025,11 @@
       <c r="D249" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249">
+        <v>7653660</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>422</v>
       </c>
@@ -4877,8 +6042,11 @@
       <c r="D250" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250">
+        <v>4661188</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>425</v>
       </c>
@@ -4891,8 +6059,11 @@
       <c r="D251" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251">
+        <v>3104974</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>427</v>
       </c>
@@ -4905,8 +6076,11 @@
       <c r="D252" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252">
+        <v>4146820</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>429</v>
       </c>
@@ -4916,8 +6090,11 @@
       <c r="C253">
         <v>-5</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>430</v>
       </c>
@@ -4930,8 +6107,11 @@
       <c r="D254" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254">
+        <v>549690</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>432</v>
       </c>
@@ -4944,8 +6124,11 @@
       <c r="D255" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255">
+        <v>1713124</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>434</v>
       </c>
@@ -4958,8 +6141,11 @@
       <c r="D256" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256">
+        <v>2558509</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>437</v>
       </c>
@@ -4972,8 +6158,11 @@
       <c r="D257" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257">
+        <v>6952311</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>439</v>
       </c>
@@ -4986,8 +6175,11 @@
       <c r="D258" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E258">
+        <v>159752</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>441</v>
       </c>
@@ -5000,8 +6192,11 @@
       <c r="D259" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259">
+        <v>2943300</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>443</v>
       </c>
@@ -5011,8 +6206,11 @@
       <c r="C260">
         <v>-1.3</v>
       </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E260" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>444</v>
       </c>
@@ -5025,8 +6223,11 @@
       <c r="D261" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E261">
+        <v>2839202</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>447</v>
       </c>
@@ -5036,8 +6237,11 @@
       <c r="C262" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E262" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>449</v>
       </c>
@@ -5047,8 +6251,11 @@
       <c r="C263">
         <v>-2.5</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E263" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>450</v>
       </c>
@@ -5061,8 +6268,11 @@
       <c r="D264" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E264">
+        <v>5660032</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>453</v>
       </c>
@@ -5072,8 +6282,11 @@
       <c r="C265">
         <v>-4.2</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E265" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>454</v>
       </c>
@@ -5086,8 +6299,11 @@
       <c r="D266" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E266">
+        <v>1536428</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>456</v>
       </c>
@@ -5099,6 +6315,14 @@
       </c>
       <c r="D267" t="s">
         <v>458</v>
+      </c>
+      <c r="E267">
+        <v>5713749</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E268" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned data with filters and got status at good speed!
</commit_message>
<xml_diff>
--- a/United_Kingdom_Banks.xlsx
+++ b/United_Kingdom_Banks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks_scrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{2810D760-9CC6-436A-B1C7-91E1A6C6C6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C7D6C4F8-8103-45A7-81A3-81F9D585D6C3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{2810D760-9CC6-436A-B1C7-91E1A6C6C6BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A21534C6-65E1-43EF-90BE-84D826706CB9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C54CCDF-854D-45B7-B0D3-70369417D37B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="583">
   <si>
     <t>Name</t>
   </si>
@@ -2150,14 +2150,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0953D09C-EEC6-4C19-A530-793F572717AA}">
   <dimension ref="A1:F267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268:XFD268"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E223" sqref="E223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2440,7 +2441,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2452,6 +2453,9 @@
       </c>
       <c r="E16" t="s">
         <v>448</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2781,7 +2785,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -2793,6 +2797,9 @@
       </c>
       <c r="E35">
         <v>7022885</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2909,7 +2916,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -2924,6 +2931,9 @@
       </c>
       <c r="E42">
         <v>4189598</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3182,7 +3192,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -3194,6 +3204,9 @@
       </c>
       <c r="E57" t="s">
         <v>471</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3233,7 +3246,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -3245,6 +3258,9 @@
       </c>
       <c r="E60" t="s">
         <v>473</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3375,7 +3391,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -3387,6 +3403,9 @@
       </c>
       <c r="E68" t="s">
         <v>478</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3443,7 +3462,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -3458,6 +3477,9 @@
       </c>
       <c r="E72" t="s">
         <v>480</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3494,7 +3516,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>137</v>
       </c>
@@ -3506,6 +3528,9 @@
       </c>
       <c r="E75" t="s">
         <v>483</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3636,7 +3661,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>148</v>
       </c>
@@ -3648,6 +3673,9 @@
       </c>
       <c r="E83" t="s">
         <v>488</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3772,7 +3800,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>159</v>
       </c>
@@ -3784,6 +3812,9 @@
       </c>
       <c r="E91" t="s">
         <v>495</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -3846,7 +3877,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>167</v>
       </c>
@@ -3861,6 +3892,9 @@
       </c>
       <c r="E95">
         <v>6621225</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -4045,7 +4079,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>185</v>
       </c>
@@ -4057,6 +4091,9 @@
       </c>
       <c r="E106" t="s">
         <v>501</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -4455,7 +4492,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>223</v>
       </c>
@@ -4470,6 +4507,9 @@
       </c>
       <c r="E128">
         <v>1814093</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -4489,7 +4529,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>226</v>
       </c>
@@ -4501,6 +4541,9 @@
       </c>
       <c r="E130" t="s">
         <v>511</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -5035,7 +5078,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>274</v>
       </c>
@@ -5047,6 +5090,9 @@
       </c>
       <c r="E160" t="s">
         <v>527</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6190,7 +6236,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>375</v>
       </c>
@@ -6202,6 +6248,9 @@
       </c>
       <c r="E223" t="s">
         <v>507</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6238,7 +6287,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>378</v>
       </c>
@@ -6250,6 +6299,9 @@
       </c>
       <c r="E226" t="s">
         <v>562</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6551,7 +6603,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>409</v>
       </c>
@@ -6563,6 +6615,9 @@
       </c>
       <c r="E243" t="s">
         <v>573</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6625,7 +6680,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>417</v>
       </c>
@@ -6640,6 +6695,9 @@
       </c>
       <c r="E247">
         <v>6952311</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6773,7 +6831,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>433</v>
       </c>
@@ -6785,6 +6843,9 @@
       </c>
       <c r="E255" t="s">
         <v>577</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6827,7 +6888,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>419</v>
       </c>
@@ -6843,8 +6904,11 @@
       <c r="E258">
         <v>159752</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F258" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>421</v>
       </c>
@@ -6860,8 +6924,11 @@
       <c r="E259">
         <v>2943300</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F259" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>423</v>
       </c>
@@ -6874,8 +6941,11 @@
       <c r="E260" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F260" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>424</v>
       </c>
@@ -6891,8 +6961,11 @@
       <c r="E261">
         <v>2839202</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F261" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>427</v>
       </c>
@@ -6905,8 +6978,11 @@
       <c r="E262" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F262" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>429</v>
       </c>
@@ -6919,8 +6995,11 @@
       <c r="E263" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F263" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>430</v>
       </c>
@@ -6936,8 +7015,11 @@
       <c r="E264">
         <v>5660032</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F264" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>433</v>
       </c>
@@ -6950,8 +7032,11 @@
       <c r="E265" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F265" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>434</v>
       </c>
@@ -6967,8 +7052,11 @@
       <c r="E266">
         <v>1536428</v>
       </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F266" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>436</v>
       </c>
@@ -6983,6 +7071,9 @@
       </c>
       <c r="E267">
         <v>5713749</v>
+      </c>
+      <c r="F267" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got uk and ireland websites
</commit_message>
<xml_diff>
--- a/United_Kingdom_Banks.xlsx
+++ b/United_Kingdom_Banks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks_scrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{386B602E-BA6B-4855-97BA-AB1E3162534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{072838D9-3954-40EE-9951-E683DC682253}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{386B602E-BA6B-4855-97BA-AB1E3162534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A4E6783-1AD8-42D2-8A36-53562B5FF3E1}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11775" xr2:uid="{33A50FC2-D249-45B2-B879-4AF1EAAC94EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{33A50FC2-D249-45B2-B879-4AF1EAAC94EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ireland" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1320">
   <si>
     <t>Name</t>
   </si>
@@ -3298,6 +3298,714 @@
   </si>
   <si>
     <t>https://find-and-update.company-information.service.gov.uk › ...</t>
+  </si>
+  <si>
+    <t>https://www.bank-abc.com › europe › London › Pages</t>
+  </si>
+  <si>
+    <t>https://www.abnamro.com</t>
+  </si>
+  <si>
+    <t>http://www.uk.abchina.com</t>
+  </si>
+  <si>
+    <t>https://aibgb.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.alrayanbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.aldermore.co.uk</t>
+  </si>
+  <si>
+    <t>https://alphabanklondon.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bank-abc.com</t>
+  </si>
+  <si>
+    <t>http://www.anb.com.sa</t>
+  </si>
+  <si>
+    <t>https://www.arbuthnotlatham.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.lhv.ee › ...</t>
+  </si>
+  <si>
+    <t>https://www.atombank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.anz.com.au › about-us</t>
+  </si>
+  <si>
+    <t>https://www.axisbankuk.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bbva.com</t>
+  </si>
+  <si>
+    <t>https://www.bradescoeuropa.eu › Ab...</t>
+  </si>
+  <si>
+    <t>https://www.bancsabadell.com › SabAtl › Particulares</t>
+  </si>
+  <si>
+    <t>https://www.bb.com.br</t>
+  </si>
+  <si>
+    <t>https://www.santander.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.bangkokbank.com › ...</t>
+  </si>
+  <si>
+    <t>https://bankandclients.com</t>
+  </si>
+  <si>
+    <t>https://www.bankleumi.co.uk</t>
+  </si>
+  <si>
+    <t>http://www.bkmandiri.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bofaml.com › dam › documents › articles</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com</t>
+  </si>
+  <si>
+    <t>https://www.bankofbaroda.in</t>
+  </si>
+  <si>
+    <t>https://www.bankofbarodauk.com</t>
+  </si>
+  <si>
+    <t>https://www.bankofbeirut.co.uk</t>
+  </si>
+  <si>
+    <t>https://bankofceylon.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bankofchina.com › uk</t>
+  </si>
+  <si>
+    <t>https://www.boc.cn › ...</t>
+  </si>
+  <si>
+    <t>https://www.hkbea.com</t>
+  </si>
+  <si>
+    <t>https://www.bankofindia.co.in</t>
+  </si>
+  <si>
+    <t>https://www.bankofirelanduk.com › about</t>
+  </si>
+  <si>
+    <t>https://www.blme.com</t>
+  </si>
+  <si>
+    <t>https://www.bmo.com › main › personal</t>
+  </si>
+  <si>
+    <t>https://www.bankofscotland.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bot.com.tw › english › pages</t>
+  </si>
+  <si>
+    <t>https://www.bpiexpressonline.com › about-bpi-europe</t>
+  </si>
+  <si>
+    <t>http://www.saderat-plc.com</t>
+  </si>
+  <si>
+    <t>http://www.banksepah.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bankingcircle.com</t>
+  </si>
+  <si>
+    <t>https://www.banquehavilland.com</t>
+  </si>
+  <si>
+    <t>https://www.banquetransatlantique.com › ...</t>
+  </si>
+  <si>
+    <t>http://bayernlb.com</t>
+  </si>
+  <si>
+    <t>https://www.bfcbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.blomfrance.com</t>
+  </si>
+  <si>
+    <t>https://www.bmce-intl.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bnf.bank</t>
+  </si>
+  <si>
+    <t>https://www.bacb.co.uk</t>
+  </si>
+  <si>
+    <t>https://brownshipley.com › en-gb</t>
+  </si>
+  <si>
+    <t>https://www.byblosbank.com › about › countries › belg...</t>
+  </si>
+  <si>
+    <t>https://www.hoaresbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://secure.cafbank.org</t>
+  </si>
+  <si>
+    <t>https://ccbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.cibc.com › personal-banking</t>
+  </si>
+  <si>
+    <t>https://www.canarabank.com</t>
+  </si>
+  <si>
+    <t>https://www.caterallen.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.dnb.com › ... › TAIWAN › TAIPEI CITY</t>
+  </si>
+  <si>
+    <t>https://chetwood.co</t>
+  </si>
+  <si>
+    <t>https://www.cncbinternational.com</t>
+  </si>
+  <si>
+    <t>http://www.uk.ccb.com</t>
+  </si>
+  <si>
+    <t>https://english.cmbchina.com</t>
+  </si>
+  <si>
+    <t>https://cibccm.com</t>
+  </si>
+  <si>
+    <t>https://www.cimb.com.my › personal</t>
+  </si>
+  <si>
+    <t>https://www.citigroup.com › citi › about › citibank_na_...</t>
+  </si>
+  <si>
+    <t>https://www.clear.bank</t>
+  </si>
+  <si>
+    <t>https://www.closebrothers.com</t>
+  </si>
+  <si>
+    <t>https://secure.cbonline.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.commerzbank.co.uk › firmenkunden › ver...</t>
+  </si>
+  <si>
+    <t>https://www.commbank.com.au</t>
+  </si>
+  <si>
+    <t>https://www.coutts.com</t>
+  </si>
+  <si>
+    <t>https://www.ca-cib.com</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org › wiki › Crédit_Industriel_et_C...</t>
+  </si>
+  <si>
+    <t>https://www.credit-suisse.com</t>
+  </si>
+  <si>
+    <t>https://www.crownagentsbank.com</t>
+  </si>
+  <si>
+    <t>https://www.cynergybank.co.uk</t>
+  </si>
+  <si>
+    <t>https://danskebank.com › about-us</t>
+  </si>
+  <si>
+    <t>https://www.dbs.com</t>
+  </si>
+  <si>
+    <t>https://www.dnb.no › ...</t>
+  </si>
+  <si>
+    <t>https://www.dzbank.com</t>
+  </si>
+  <si>
+    <t>https://www.efgl.com</t>
+  </si>
+  <si>
+    <t>https://www.emiratesnbd.com › company-details</t>
+  </si>
+  <si>
+    <t>https://www.erstegroup.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.eurobankpb.lu › Home › About us</t>
+  </si>
+  <si>
+    <t>https://www.eabplc.com</t>
+  </si>
+  <si>
+    <t>https://www.fbnbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.fcebank.com</t>
+  </si>
+  <si>
+    <t>https://www.fcmbuk.com</t>
+  </si>
+  <si>
+    <t>https://www.bankfab.com › en-ae › about-fab</t>
+  </si>
+  <si>
+    <t>https://www.1cb.com</t>
+  </si>
+  <si>
+    <t>https://www.firstrand.co.za</t>
+  </si>
+  <si>
+    <t>https://www.ghanabank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.goldmansachs.com › what-we-do › consu...</t>
+  </si>
+  <si>
+    <t>https://www.gtbankuk.com</t>
+  </si>
+  <si>
+    <t>https://www.habibbank.com</t>
+  </si>
+  <si>
+    <t>https://www.hbl.com</t>
+  </si>
+  <si>
+    <t>https://www.habibbank.com › home › ukHome</t>
+  </si>
+  <si>
+    <t>https://www.hampdenandco.com</t>
+  </si>
+  <si>
+    <t>https://www.htb.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.handelsbanken.co.uk › ...</t>
+  </si>
+  <si>
+    <t>https://www.hauck-aufhaeuser.com › ...</t>
+  </si>
+  <si>
+    <t>http://www.havanaintbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://hblbankuk.com</t>
+  </si>
+  <si>
+    <t>https://www.hsbc.co.uk</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu › ... › United Kingdom</t>
+  </si>
+  <si>
+    <t>https://www.icbclondon.com</t>
+  </si>
+  <si>
+    <t>https://www.icbcstandardbank.com</t>
+  </si>
+  <si>
+    <t>https://www.icicibank.co.uk</t>
+  </si>
+  <si>
+    <t>https://ikano.co.uk</t>
+  </si>
+  <si>
+    <t>http://www.icbc-ltd.com › icbcltd</t>
+  </si>
+  <si>
+    <t>https://global.ibk.co.kr</t>
+  </si>
+  <si>
+    <t>http://intesasanpaolo.com</t>
+  </si>
+  <si>
+    <t>https://www.itau.com.br › itaubba-en › international</t>
+  </si>
+  <si>
+    <t>https://www.jordanbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.jpmorganchase.com</t>
+  </si>
+  <si>
+    <t>https://www.kbc.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.kebhana.com › easyone_index_en</t>
+  </si>
+  <si>
+    <t>https://www.kfw-ipex-bank.de › International-financing</t>
+  </si>
+  <si>
+    <t>https://www.kingdom.bank</t>
+  </si>
+  <si>
+    <t>https://www.kbfg.com › about › global › europe › list</t>
+  </si>
+  <si>
+    <t>https://www.lbbw.de › homepage</t>
+  </si>
+  <si>
+    <t>https://www.helaba.com</t>
+  </si>
+  <si>
+    <t>https://www.lloydsbank.com › important-information</t>
+  </si>
+  <si>
+    <t>https://www.lloydsbank.com</t>
+  </si>
+  <si>
+    <t>https://www.lombardodier.com › ... › luxembourg.</t>
+  </si>
+  <si>
+    <t>https://www.macquarie.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.maybank.com</t>
+  </si>
+  <si>
+    <t>https://bank.marksandspencer.com</t>
+  </si>
+  <si>
+    <t>https://mashreqbank.com</t>
+  </si>
+  <si>
+    <t>https://www.masthaven.co.uk › Home</t>
+  </si>
+  <si>
+    <t>https://www.megabank.com.tw › en-us › english</t>
+  </si>
+  <si>
+    <t>https://www.mellibank.com</t>
+  </si>
+  <si>
+    <t>https://www.mcafundingforchurches.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.metrobankonline.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.tr.mufg.jp › english</t>
+  </si>
+  <si>
+    <t>https://www.mizrahi-tefahot.co.il › ...</t>
+  </si>
+  <si>
+    <t>https://www.mizuhogroup.com › bank</t>
+  </si>
+  <si>
+    <t>https://www.mizuhogroup.com › emea</t>
+  </si>
+  <si>
+    <t>https://www.monument.co</t>
+  </si>
+  <si>
+    <t>https://monzo.com</t>
+  </si>
+  <si>
+    <t>https://www.morganstanley.com › global-offices › unite...</t>
+  </si>
+  <si>
+    <t>https://www.bk.mufg.jp › global</t>
+  </si>
+  <si>
+    <t>https://n26.com › en-gb</t>
+  </si>
+  <si>
+    <t>https://www.nab.com.au</t>
+  </si>
+  <si>
+    <t>https://www.nbeuk.com</t>
+  </si>
+  <si>
+    <t>https://www.nbg.gr › ...</t>
+  </si>
+  <si>
+    <t>https://www.nbk.com › london › About</t>
+  </si>
+  <si>
+    <t>https://personal.natwest.com › personal</t>
+  </si>
+  <si>
+    <t>https://www.natixis.com › natixis › home-j_6</t>
+  </si>
+  <si>
+    <t>https://www.nedbank.co.za › desktop › personal</t>
+  </si>
+  <si>
+    <t>https://nedbankprivatewealth.com</t>
+  </si>
+  <si>
+    <t>https://www.nomura.com</t>
+  </si>
+  <si>
+    <t>https://www.nordlb.de</t>
+  </si>
+  <si>
+    <t>https://www.nordea.com › debt-and-rating › Prospectuses</t>
+  </si>
+  <si>
+    <t>https://www.ocbc.com › group › gateway</t>
+  </si>
+  <si>
+    <t>https://www.paragonbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://pcf.bank</t>
+  </si>
+  <si>
+    <t>http://www.persiabank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.pnb.com.ph › europe</t>
+  </si>
+  <si>
+    <t>https://www.piraeusholdings.gr › ...</t>
+  </si>
+  <si>
+    <t>https://www.bni.co.id › id-id</t>
+  </si>
+  <si>
+    <t>https://www.pnbint.com</t>
+  </si>
+  <si>
+    <t>https://www.qnb.com</t>
+  </si>
+  <si>
+    <t>https://www.qib-uk.com</t>
+  </si>
+  <si>
+    <t>https://www.raphaelsbank.com</t>
+  </si>
+  <si>
+    <t>https://www.rbinternational.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.rcibank.co.uk</t>
+  </si>
+  <si>
+    <t>https://redwoodbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.reliancebankltd.com</t>
+  </si>
+  <si>
+    <t>https://www.riyadbank.com › personal-banking</t>
+  </si>
+  <si>
+    <t>http://www.rbcroyalbank.com</t>
+  </si>
+  <si>
+    <t>https://www.sainsburysbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.santander.co.uk › ... › Investor relations</t>
+  </si>
+  <si>
+    <t>https://www.santander.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.securetrustbank.com</t>
+  </si>
+  <si>
+    <t>https://www.kleinworthambros.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.shacombank.com.hk › eng › personal</t>
+  </si>
+  <si>
+    <t>https://www.sigchina.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.shawbrook.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.shinhan.com › ...</t>
+  </si>
+  <si>
+    <t>https://sebgroup.com</t>
+  </si>
+  <si>
+    <t>https://www.societegenerale.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.sonali-bank.com</t>
+  </si>
+  <si>
+    <t>https://www.sc.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.starlingbank.com</t>
+  </si>
+  <si>
+    <t>https://www.statestreet.com › bank-and-trust-policies</t>
+  </si>
+  <si>
+    <t>https://www.statestreet.com › about › office-locations</t>
+  </si>
+  <si>
+    <t>https://www.stifel.com › stifel-europe › seba-disclosures</t>
+  </si>
+  <si>
+    <t>https://www.smbcgroup.com › emea</t>
+  </si>
+  <si>
+    <t>https://syndicatebank.in</t>
+  </si>
+  <si>
+    <t>https://www.ziraatbank.com.tr › ...</t>
+  </si>
+  <si>
+    <t>https://www.tandem.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.tescobank.com</t>
+  </si>
+  <si>
+    <t>https://www.theaccessbankukltd.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bnymellon.com</t>
+  </si>
+  <si>
+    <t>https://www.scotiabank.com › global › global-site</t>
+  </si>
+  <si>
+    <t>https://charitybank.org</t>
+  </si>
+  <si>
+    <t>https://www.chibabank.co.jp › english</t>
+  </si>
+  <si>
+    <t>https://www.co-operativebank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.bankofengland.co.uk › knowledgebank</t>
+  </si>
+  <si>
+    <t>https://www.bankofireland.com › press-releases › the-g...</t>
+  </si>
+  <si>
+    <t>https://www.hsbc.com.hk</t>
+  </si>
+  <si>
+    <t>https://www.kdb.co.kr › hmp › CHGMLO1300.html</t>
+  </si>
+  <si>
+    <t>https://www.nochubank.or.jp › ...</t>
+  </si>
+  <si>
+    <t>https://www.rbsinternational.com</t>
+  </si>
+  <si>
+    <t>https://personal.rbs.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.td.com › personal-banking</t>
+  </si>
+  <si>
+    <t>https://www.triodos.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.tsb.co.uk › personal</t>
+  </si>
+  <si>
+    <t>https://www.turkishbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.isbank.com.tr › ...</t>
+  </si>
+  <si>
+    <t>https://www.ubs.com › global</t>
+  </si>
+  <si>
+    <t>https://digital.ulsterbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.unicreditgroup.eu › ... › Europe › Germany</t>
+  </si>
+  <si>
+    <t>https://www.unicreditgroup.eu › ... › Europe › Italy</t>
+  </si>
+  <si>
+    <t>https://www.ubp.com › ...</t>
+  </si>
+  <si>
+    <t>https://www.unionbankofindiauk.co.uk</t>
+  </si>
+  <si>
+    <t>http://www.unionbankuk.com</t>
+  </si>
+  <si>
+    <t>https://www.ubauk.com</t>
+  </si>
+  <si>
+    <t>https://www.ubluk.com</t>
+  </si>
+  <si>
+    <t>https://www.uobgroup.com › uobgroup</t>
+  </si>
+  <si>
+    <t>https://www.utbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.unity.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.vanquis.co.uk</t>
+  </si>
+  <si>
+    <t>https://uk.virginmoney.com</t>
+  </si>
+  <si>
+    <t>https://www.vtbcapital.com</t>
+  </si>
+  <si>
+    <t>https://www.weatherbys.bank</t>
+  </si>
+  <si>
+    <t>https://www.wellsfargo.com</t>
+  </si>
+  <si>
+    <t>https://www.wesleyan.co.uk › wesleyan-bank</t>
+  </si>
+  <si>
+    <t>https://www.westernunion.com › western-union-bank</t>
+  </si>
+  <si>
+    <t>https://www.westpac.com.au</t>
+  </si>
+  <si>
+    <t>https://www.westpac.com.au › ... › Global locations</t>
+  </si>
+  <si>
+    <t>http://eng.wooribank.com</t>
+  </si>
+  <si>
+    <t>https://www.wyelandsbank.co.uk</t>
+  </si>
+  <si>
+    <t>https://www.zenith-bank.co.uk</t>
   </si>
 </sst>
 </file>
@@ -3658,7 +4366,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4910,7 +5624,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3D35A5-D059-4ACF-842D-672F158C38D5}">
-  <dimension ref="A1:G267"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -4921,9 +5635,10 @@
     <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4945,8 +5660,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4968,8 +5686,11 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -4988,8 +5709,11 @@
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -5008,8 +5732,11 @@
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -5031,8 +5758,11 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -5054,8 +5784,11 @@
       <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -5077,8 +5810,11 @@
       <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -5100,8 +5836,11 @@
       <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -5120,8 +5859,11 @@
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -5140,8 +5882,11 @@
       <c r="G10" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5163,8 +5908,11 @@
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -5183,8 +5931,11 @@
       <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -5206,8 +5957,11 @@
       <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -5226,8 +5980,11 @@
       <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -5249,8 +6006,11 @@
       <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -5269,8 +6029,11 @@
       <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -5289,8 +6052,11 @@
       <c r="G17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -5309,8 +6075,11 @@
       <c r="G18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -5329,8 +6098,11 @@
       <c r="G19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -5349,8 +6121,11 @@
       <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -5369,8 +6144,11 @@
       <c r="G21" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -5392,8 +6170,11 @@
       <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -5415,8 +6196,11 @@
       <c r="G23" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -5438,8 +6222,11 @@
       <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -5458,8 +6245,11 @@
       <c r="G25" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -5478,8 +6268,11 @@
       <c r="G26" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -5495,8 +6288,11 @@
       <c r="G27" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -5518,8 +6314,11 @@
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -5541,8 +6340,11 @@
       <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -5564,8 +6366,11 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -5587,8 +6392,11 @@
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>117</v>
       </c>
@@ -5607,8 +6415,11 @@
       <c r="G32" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -5627,8 +6438,11 @@
       <c r="G33" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -5647,8 +6461,11 @@
       <c r="G34" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>126</v>
       </c>
@@ -5667,8 +6484,11 @@
       <c r="G35" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -5687,8 +6507,11 @@
       <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>131</v>
       </c>
@@ -5710,8 +6533,11 @@
       <c r="G37" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>135</v>
       </c>
@@ -5730,8 +6556,11 @@
       <c r="G38" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -5753,8 +6582,11 @@
       <c r="G39" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>143</v>
       </c>
@@ -5773,8 +6605,11 @@
       <c r="G40" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -5796,8 +6631,11 @@
       <c r="G41" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -5819,8 +6657,11 @@
       <c r="G42" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>153</v>
       </c>
@@ -5842,8 +6683,11 @@
       <c r="G43" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>156</v>
       </c>
@@ -5862,8 +6706,11 @@
       <c r="G44" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>160</v>
       </c>
@@ -5882,8 +6729,11 @@
       <c r="G45" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>164</v>
       </c>
@@ -5902,8 +6752,11 @@
       <c r="G46" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>168</v>
       </c>
@@ -5925,8 +6778,11 @@
       <c r="G47" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>170</v>
       </c>
@@ -5948,8 +6804,11 @@
       <c r="G48" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>173</v>
       </c>
@@ -5968,8 +6827,11 @@
       <c r="G49" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>176</v>
       </c>
@@ -5991,8 +6853,11 @@
       <c r="G50" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -6011,8 +6876,11 @@
       <c r="G51" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>182</v>
       </c>
@@ -6034,8 +6902,11 @@
       <c r="G52" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>185</v>
       </c>
@@ -6054,8 +6925,11 @@
       <c r="G53" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>188</v>
       </c>
@@ -6074,8 +6948,11 @@
       <c r="G54" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>191</v>
       </c>
@@ -6097,8 +6974,11 @@
       <c r="G55" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>194</v>
       </c>
@@ -6120,8 +7000,11 @@
       <c r="G56" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -6140,8 +7023,11 @@
       <c r="G57" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>200</v>
       </c>
@@ -6163,8 +7049,11 @@
       <c r="G58" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>203</v>
       </c>
@@ -6186,8 +7075,11 @@
       <c r="G59" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>207</v>
       </c>
@@ -6209,8 +7101,11 @@
       <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>209</v>
       </c>
@@ -6229,8 +7124,11 @@
       <c r="G61" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>212</v>
       </c>
@@ -6249,8 +7147,11 @@
       <c r="G62" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -6272,8 +7173,11 @@
       <c r="G63" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>217</v>
       </c>
@@ -6292,8 +7196,11 @@
       <c r="G64" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>220</v>
       </c>
@@ -6315,8 +7222,11 @@
       <c r="G65" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>223</v>
       </c>
@@ -6335,8 +7245,11 @@
       <c r="G66" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>226</v>
       </c>
@@ -6358,8 +7271,11 @@
       <c r="G67" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>229</v>
       </c>
@@ -6378,8 +7294,11 @@
       <c r="G68" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -6398,8 +7317,11 @@
       <c r="G69" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>235</v>
       </c>
@@ -6421,8 +7343,11 @@
       <c r="G70" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>239</v>
       </c>
@@ -6441,8 +7366,11 @@
       <c r="G71" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>242</v>
       </c>
@@ -6461,8 +7389,11 @@
       <c r="G72" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>244</v>
       </c>
@@ -6481,8 +7412,11 @@
       <c r="G73" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>247</v>
       </c>
@@ -6501,8 +7435,11 @@
       <c r="G74" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>250</v>
       </c>
@@ -6524,8 +7461,11 @@
       <c r="G75" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>254</v>
       </c>
@@ -6547,8 +7487,11 @@
       <c r="G76" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>258</v>
       </c>
@@ -6567,8 +7510,11 @@
       <c r="G77" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>261</v>
       </c>
@@ -6587,8 +7533,11 @@
       <c r="G78" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>264</v>
       </c>
@@ -6607,8 +7556,11 @@
       <c r="G79" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>267</v>
       </c>
@@ -6630,8 +7582,11 @@
       <c r="G80" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>269</v>
       </c>
@@ -6650,8 +7605,11 @@
       <c r="G81" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>272</v>
       </c>
@@ -6670,8 +7628,11 @@
       <c r="G82" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>275</v>
       </c>
@@ -6690,8 +7651,11 @@
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -6713,8 +7677,11 @@
       <c r="G84" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>281</v>
       </c>
@@ -6736,8 +7703,11 @@
       <c r="G85" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>284</v>
       </c>
@@ -6759,8 +7729,11 @@
       <c r="G86" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>287</v>
       </c>
@@ -6779,8 +7752,11 @@
       <c r="G87" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>290</v>
       </c>
@@ -6799,8 +7775,11 @@
       <c r="G88" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>293</v>
       </c>
@@ -6819,8 +7798,11 @@
       <c r="G89" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>296</v>
       </c>
@@ -6839,8 +7821,11 @@
       <c r="G90" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>299</v>
       </c>
@@ -6859,8 +7844,11 @@
       <c r="G91" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>302</v>
       </c>
@@ -6882,8 +7870,11 @@
       <c r="G92" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>306</v>
       </c>
@@ -6902,8 +7893,11 @@
       <c r="G93" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>311</v>
       </c>
@@ -6922,8 +7916,11 @@
       <c r="G94" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>314</v>
       </c>
@@ -6942,8 +7939,11 @@
       <c r="G95" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>317</v>
       </c>
@@ -6962,8 +7962,11 @@
       <c r="G96" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>320</v>
       </c>
@@ -6985,8 +7988,11 @@
       <c r="G97" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>322</v>
       </c>
@@ -7008,8 +8014,11 @@
       <c r="G98" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>325</v>
       </c>
@@ -7031,8 +8040,11 @@
       <c r="G99" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>329</v>
       </c>
@@ -7054,8 +8066,11 @@
       <c r="G100" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>332</v>
       </c>
@@ -7077,8 +8092,11 @@
       <c r="G101" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>335</v>
       </c>
@@ -7097,8 +8115,11 @@
       <c r="G102" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>338</v>
       </c>
@@ -7117,8 +8138,11 @@
       <c r="G103" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>341</v>
       </c>
@@ -7137,8 +8161,11 @@
       <c r="G104" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>344</v>
       </c>
@@ -7157,8 +8184,11 @@
       <c r="G105" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>347</v>
       </c>
@@ -7180,8 +8210,11 @@
       <c r="G106" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>351</v>
       </c>
@@ -7200,8 +8233,11 @@
       <c r="G107" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>354</v>
       </c>
@@ -7223,8 +8259,11 @@
       <c r="G108" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>357</v>
       </c>
@@ -7246,8 +8285,11 @@
       <c r="G109" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>360</v>
       </c>
@@ -7266,8 +8308,11 @@
       <c r="G110" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>362</v>
       </c>
@@ -7286,8 +8331,11 @@
       <c r="G111" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>365</v>
       </c>
@@ -7309,8 +8357,11 @@
       <c r="G112" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>368</v>
       </c>
@@ -7332,8 +8383,11 @@
       <c r="G113" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>370</v>
       </c>
@@ -7355,8 +8409,11 @@
       <c r="G114" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>374</v>
       </c>
@@ -7378,8 +8435,11 @@
       <c r="G115" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>377</v>
       </c>
@@ -7398,8 +8458,11 @@
       <c r="G116" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>378</v>
       </c>
@@ -7421,8 +8484,11 @@
       <c r="G117" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>382</v>
       </c>
@@ -7444,8 +8510,11 @@
       <c r="G118" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>385</v>
       </c>
@@ -7467,8 +8536,11 @@
       <c r="G119" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>388</v>
       </c>
@@ -7487,8 +8559,11 @@
       <c r="G120" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>391</v>
       </c>
@@ -7510,8 +8585,11 @@
       <c r="G121" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>394</v>
       </c>
@@ -7533,8 +8611,11 @@
       <c r="G122" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>397</v>
       </c>
@@ -7553,8 +8634,11 @@
       <c r="G123" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>400</v>
       </c>
@@ -7576,8 +8660,11 @@
       <c r="G124" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>403</v>
       </c>
@@ -7599,8 +8686,11 @@
       <c r="G125" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>406</v>
       </c>
@@ -7622,8 +8712,11 @@
       <c r="G126" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>409</v>
       </c>
@@ -7642,8 +8735,11 @@
       <c r="G127" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>412</v>
       </c>
@@ -7662,8 +8758,11 @@
       <c r="G128" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>415</v>
       </c>
@@ -7682,8 +8781,11 @@
       <c r="G129" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>418</v>
       </c>
@@ -7702,8 +8804,11 @@
       <c r="G130" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>422</v>
       </c>
@@ -7722,8 +8827,11 @@
       <c r="G131" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>425</v>
       </c>
@@ -7745,8 +8853,11 @@
       <c r="G132" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>428</v>
       </c>
@@ -7765,8 +8876,11 @@
       <c r="G133" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>431</v>
       </c>
@@ -7788,8 +8902,11 @@
       <c r="G134" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>434</v>
       </c>
@@ -7811,8 +8928,11 @@
       <c r="G135" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>437</v>
       </c>
@@ -7831,8 +8951,11 @@
       <c r="G136" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>440</v>
       </c>
@@ -7851,8 +8974,11 @@
       <c r="G137" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>443</v>
       </c>
@@ -7871,8 +8997,11 @@
       <c r="G138" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>446</v>
       </c>
@@ -7894,8 +9023,11 @@
       <c r="G139" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>449</v>
       </c>
@@ -7914,8 +9046,11 @@
       <c r="G140" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>452</v>
       </c>
@@ -7937,8 +9072,11 @@
       <c r="G141" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>456</v>
       </c>
@@ -7957,8 +9095,11 @@
       <c r="G142" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>459</v>
       </c>
@@ -7977,8 +9118,11 @@
       <c r="G143" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>462</v>
       </c>
@@ -7997,8 +9141,11 @@
       <c r="G144" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>465</v>
       </c>
@@ -8020,8 +9167,11 @@
       <c r="G145" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>468</v>
       </c>
@@ -8043,8 +9193,11 @@
       <c r="G146" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>471</v>
       </c>
@@ -8063,8 +9216,11 @@
       <c r="G147" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>474</v>
       </c>
@@ -8086,8 +9242,11 @@
       <c r="G148" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>478</v>
       </c>
@@ -8106,8 +9265,11 @@
       <c r="G149" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>480</v>
       </c>
@@ -8129,8 +9291,11 @@
       <c r="G150" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>483</v>
       </c>
@@ -8149,8 +9314,11 @@
       <c r="G151" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>486</v>
       </c>
@@ -8172,8 +9340,11 @@
       <c r="G152" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>488</v>
       </c>
@@ -8192,8 +9363,11 @@
       <c r="G153" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>491</v>
       </c>
@@ -8215,8 +9389,11 @@
       <c r="G154" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>494</v>
       </c>
@@ -8235,8 +9412,11 @@
       <c r="G155" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H155" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>497</v>
       </c>
@@ -8258,8 +9438,11 @@
       <c r="G156" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H156" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>500</v>
       </c>
@@ -8281,8 +9464,11 @@
       <c r="G157" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H157" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>503</v>
       </c>
@@ -8304,8 +9490,11 @@
       <c r="G158" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H158" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>506</v>
       </c>
@@ -8324,8 +9513,11 @@
       <c r="G159" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H159" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>510</v>
       </c>
@@ -8344,8 +9536,11 @@
       <c r="G160" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H160" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>514</v>
       </c>
@@ -8364,8 +9559,11 @@
       <c r="G161" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H161" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>517</v>
       </c>
@@ -8387,8 +9585,11 @@
       <c r="G162" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H162" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>519</v>
       </c>
@@ -8407,8 +9608,11 @@
       <c r="G163" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H163" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>521</v>
       </c>
@@ -8430,8 +9634,11 @@
       <c r="G164" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>524</v>
       </c>
@@ -8453,8 +9660,11 @@
       <c r="G165" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H165" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>528</v>
       </c>
@@ -8473,8 +9683,11 @@
       <c r="G166" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H166" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>531</v>
       </c>
@@ -8493,8 +9706,11 @@
       <c r="G167" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H167" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>534</v>
       </c>
@@ -8513,8 +9729,11 @@
       <c r="G168" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H168" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>537</v>
       </c>
@@ -8536,8 +9755,11 @@
       <c r="G169" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H169" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>540</v>
       </c>
@@ -8556,8 +9778,11 @@
       <c r="G170" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H170" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>543</v>
       </c>
@@ -8579,8 +9804,11 @@
       <c r="G171" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H171" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>546</v>
       </c>
@@ -8602,8 +9830,11 @@
       <c r="G172" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H172" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>549</v>
       </c>
@@ -8622,8 +9853,11 @@
       <c r="G173" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H173" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>552</v>
       </c>
@@ -8642,8 +9876,11 @@
       <c r="G174" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H174" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>555</v>
       </c>
@@ -8662,8 +9899,11 @@
       <c r="G175" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H175" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>558</v>
       </c>
@@ -8685,8 +9925,11 @@
       <c r="G176" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H176" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>561</v>
       </c>
@@ -8705,8 +9948,11 @@
       <c r="G177" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H177" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>564</v>
       </c>
@@ -8725,8 +9971,11 @@
       <c r="G178" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H178" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>567</v>
       </c>
@@ -8748,8 +9997,11 @@
       <c r="G179" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H179" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>572</v>
       </c>
@@ -8768,8 +10020,11 @@
       <c r="G180" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H180" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>575</v>
       </c>
@@ -8791,8 +10046,11 @@
       <c r="G181" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H181" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>578</v>
       </c>
@@ -8814,8 +10072,11 @@
       <c r="G182" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H182" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>581</v>
       </c>
@@ -8837,8 +10098,11 @@
       <c r="G183" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H183" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>584</v>
       </c>
@@ -8860,8 +10124,11 @@
       <c r="G184" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H184" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>587</v>
       </c>
@@ -8880,8 +10147,11 @@
       <c r="G185" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H185" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>590</v>
       </c>
@@ -8900,8 +10170,11 @@
       <c r="G186" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H186" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>593</v>
       </c>
@@ -8923,8 +10196,11 @@
       <c r="G187" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H187" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>596</v>
       </c>
@@ -8943,8 +10219,11 @@
       <c r="G188" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>599</v>
       </c>
@@ -8966,8 +10245,11 @@
       <c r="G189" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H189" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>603</v>
       </c>
@@ -8989,8 +10271,11 @@
       <c r="G190" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H190" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>605</v>
       </c>
@@ -9009,8 +10294,11 @@
       <c r="G191" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H191" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>608</v>
       </c>
@@ -9032,8 +10320,11 @@
       <c r="G192" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H192" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>611</v>
       </c>
@@ -9052,8 +10343,11 @@
       <c r="G193" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H193" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>613</v>
       </c>
@@ -9075,8 +10369,11 @@
       <c r="G194" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H194" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>617</v>
       </c>
@@ -9098,8 +10395,11 @@
       <c r="G195" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H195" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>620</v>
       </c>
@@ -9118,8 +10418,11 @@
       <c r="G196" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H196" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>624</v>
       </c>
@@ -9138,8 +10441,11 @@
       <c r="G197" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H197" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>626</v>
       </c>
@@ -9161,8 +10467,11 @@
       <c r="G198" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H198" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>628</v>
       </c>
@@ -9184,8 +10493,11 @@
       <c r="G199" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H199" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>631</v>
       </c>
@@ -9207,8 +10519,11 @@
       <c r="G200" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H200" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>633</v>
       </c>
@@ -9230,8 +10545,11 @@
       <c r="G201" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H201" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>636</v>
       </c>
@@ -9253,8 +10571,11 @@
       <c r="G202" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H202" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>639</v>
       </c>
@@ -9276,8 +10597,11 @@
       <c r="G203" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H203" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>642</v>
       </c>
@@ -9296,8 +10620,11 @@
       <c r="G204" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H204" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>645</v>
       </c>
@@ -9316,8 +10643,11 @@
       <c r="G205" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H205" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>648</v>
       </c>
@@ -9339,8 +10669,11 @@
       <c r="G206" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H206" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>651</v>
       </c>
@@ -9359,8 +10692,11 @@
       <c r="G207" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H207" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>654</v>
       </c>
@@ -9379,8 +10715,11 @@
       <c r="G208" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H208" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>656</v>
       </c>
@@ -9399,8 +10738,11 @@
       <c r="G209" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H209" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>658</v>
       </c>
@@ -9419,8 +10761,11 @@
       <c r="G210" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H210" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>661</v>
       </c>
@@ -9442,8 +10787,11 @@
       <c r="G211" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H211" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>665</v>
       </c>
@@ -9465,8 +10813,11 @@
       <c r="G212" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H212" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>669</v>
       </c>
@@ -9488,8 +10839,11 @@
       <c r="G213" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H213" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>672</v>
       </c>
@@ -9508,8 +10862,11 @@
       <c r="G214" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H214" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>675</v>
       </c>
@@ -9528,8 +10885,11 @@
       <c r="G215" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H215" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>678</v>
       </c>
@@ -9548,8 +10908,11 @@
       <c r="G216" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H216" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>680</v>
       </c>
@@ -9568,8 +10931,11 @@
       <c r="G217" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H217" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>683</v>
       </c>
@@ -9588,8 +10954,11 @@
       <c r="G218" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H218" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>685</v>
       </c>
@@ -9608,8 +10977,11 @@
       <c r="G219" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H219" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>688</v>
       </c>
@@ -9628,8 +11000,11 @@
       <c r="G220" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H220" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>691</v>
       </c>
@@ -9651,8 +11026,11 @@
       <c r="G221" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H221" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>694</v>
       </c>
@@ -9674,8 +11052,11 @@
       <c r="G222" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H222" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>697</v>
       </c>
@@ -9697,8 +11078,11 @@
       <c r="G223" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H223" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>701</v>
       </c>
@@ -9720,8 +11104,11 @@
       <c r="G224" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H224" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>705</v>
       </c>
@@ -9740,8 +11127,11 @@
       <c r="G225" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H225" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>708</v>
       </c>
@@ -9763,8 +11153,11 @@
       <c r="G226" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H226" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>711</v>
       </c>
@@ -9783,8 +11176,11 @@
       <c r="G227" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H227" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>713</v>
       </c>
@@ -9803,8 +11199,11 @@
       <c r="G228" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H228" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>716</v>
       </c>
@@ -9826,8 +11225,11 @@
       <c r="G229" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H229" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>720</v>
       </c>
@@ -9846,8 +11248,11 @@
       <c r="G230" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H230" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>723</v>
       </c>
@@ -9869,8 +11274,11 @@
       <c r="G231" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H231" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>725</v>
       </c>
@@ -9886,8 +11294,11 @@
       <c r="F232" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H232" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>729</v>
       </c>
@@ -9906,8 +11317,11 @@
       <c r="G233" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H233" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>731</v>
       </c>
@@ -9926,8 +11340,11 @@
       <c r="G234" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H234" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>734</v>
       </c>
@@ -9946,8 +11363,11 @@
       <c r="G235" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H235" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>737</v>
       </c>
@@ -9966,8 +11386,11 @@
       <c r="G236" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H236" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>741</v>
       </c>
@@ -9986,8 +11409,11 @@
       <c r="G237" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H237" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>745</v>
       </c>
@@ -10009,8 +11435,11 @@
       <c r="G238" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H238" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>749</v>
       </c>
@@ -10029,8 +11458,11 @@
       <c r="G239" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H239" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>752</v>
       </c>
@@ -10052,8 +11484,11 @@
       <c r="G240" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H240" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>756</v>
       </c>
@@ -10075,8 +11510,11 @@
       <c r="G241" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H241" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>760</v>
       </c>
@@ -10098,8 +11536,11 @@
       <c r="G242" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H242" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>763</v>
       </c>
@@ -10118,8 +11559,11 @@
       <c r="G243" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H243" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>766</v>
       </c>
@@ -10138,8 +11582,11 @@
       <c r="G244" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H244" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>769</v>
       </c>
@@ -10161,8 +11608,11 @@
       <c r="G245" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H245" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>772</v>
       </c>
@@ -10181,8 +11631,11 @@
       <c r="G246" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H246" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>775</v>
       </c>
@@ -10201,8 +11654,11 @@
       <c r="G247" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H247" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>778</v>
       </c>
@@ -10221,8 +11677,11 @@
       <c r="G248" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H248" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>782</v>
       </c>
@@ -10244,8 +11703,11 @@
       <c r="G249" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H249" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>785</v>
       </c>
@@ -10267,8 +11729,11 @@
       <c r="G250" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H250" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>789</v>
       </c>
@@ -10290,8 +11755,11 @@
       <c r="G251" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H251" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>791</v>
       </c>
@@ -10313,8 +11781,11 @@
       <c r="G252" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H252" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>794</v>
       </c>
@@ -10333,8 +11804,11 @@
       <c r="G253" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H253" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>797</v>
       </c>
@@ -10356,8 +11830,11 @@
       <c r="G254" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H254" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>800</v>
       </c>
@@ -10379,8 +11856,11 @@
       <c r="G255" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H255" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>803</v>
       </c>
@@ -10402,8 +11882,11 @@
       <c r="G256" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>807</v>
       </c>
@@ -10425,8 +11908,11 @@
       <c r="G257" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H257" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>810</v>
       </c>
@@ -10448,8 +11934,11 @@
       <c r="G258" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H258" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>813</v>
       </c>
@@ -10471,8 +11960,11 @@
       <c r="G259" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H259" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>816</v>
       </c>
@@ -10491,8 +11983,11 @@
       <c r="G260" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H260" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>819</v>
       </c>
@@ -10514,8 +12009,11 @@
       <c r="G261" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="262" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H261" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>822</v>
       </c>
@@ -10534,8 +12032,11 @@
       <c r="G262" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="263" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H262" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>826</v>
       </c>
@@ -10554,8 +12055,11 @@
       <c r="G263" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="264" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H263" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>829</v>
       </c>
@@ -10577,8 +12081,11 @@
       <c r="G264" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="265" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H264" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>832</v>
       </c>
@@ -10597,8 +12104,11 @@
       <c r="G265" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="266" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H265" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>835</v>
       </c>
@@ -10620,8 +12130,11 @@
       <c r="G266" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="267" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H266" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>838</v>
       </c>
@@ -10642,6 +12155,9 @@
       </c>
       <c r="G267" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H267" t="s">
+        <v>1319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished the cayman islands
</commit_message>
<xml_diff>
--- a/United_Kingdom_Banks.xlsx
+++ b/United_Kingdom_Banks.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks_scrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{386B602E-BA6B-4855-97BA-AB1E3162534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A4E6783-1AD8-42D2-8A36-53562B5FF3E1}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{386B602E-BA6B-4855-97BA-AB1E3162534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB1C1926-2069-431A-9F5A-8DC0D6559A00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{33A50FC2-D249-45B2-B879-4AF1EAAC94EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ireland" sheetId="2" r:id="rId1"/>
-    <sheet name="United Kingdom" sheetId="1" r:id="rId2"/>
+    <sheet name="Cayman" sheetId="3" r:id="rId1"/>
+    <sheet name="Ireland" sheetId="2" r:id="rId2"/>
+    <sheet name="United Kingdom" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'United Kingdom'!$A$1:$G$267</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'United Kingdom'!$A$1:$G$267</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2721" uniqueCount="1618">
   <si>
     <t>Name</t>
   </si>
@@ -4006,6 +4007,900 @@
   </si>
   <si>
     <t>https://www.zenith-bank.co.uk</t>
+  </si>
+  <si>
+    <t>Alexandria Bancorp Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18104</t>
+  </si>
+  <si>
+    <t>banking and trustee services</t>
+  </si>
+  <si>
+    <t>international only</t>
+  </si>
+  <si>
+    <t>https://www.alexandriabancorp.com</t>
+  </si>
+  <si>
+    <t>Alhambra Bank &amp; Trust Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18589</t>
+  </si>
+  <si>
+    <t>http://alhambrabank.ky</t>
+  </si>
+  <si>
+    <t>Altajir Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18106</t>
+  </si>
+  <si>
+    <t>http://www.altajirbank.com</t>
+  </si>
+  <si>
+    <t>American Express National Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18108</t>
+  </si>
+  <si>
+    <t>banking services</t>
+  </si>
+  <si>
+    <t>https://www.americanexpress.com › en-us › banking</t>
+  </si>
+  <si>
+    <t>Atlantic Security Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18110</t>
+  </si>
+  <si>
+    <t>https://www.asbnet.com</t>
+  </si>
+  <si>
+    <t>Australia and New Zealand Banking Group Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18111</t>
+  </si>
+  <si>
+    <t>BAC International Bank (Grand Cayman)</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18112</t>
+  </si>
+  <si>
+    <t>https://cayman.directory › bac-international-bank-grand...</t>
+  </si>
+  <si>
+    <t>Banco ABC Brasil S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18113</t>
+  </si>
+  <si>
+    <t>https://www.abcbrasil.com.br › who-we-are</t>
+  </si>
+  <si>
+    <t>Banco Bradesco S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18117</t>
+  </si>
+  <si>
+    <t>https://banco.bradesco</t>
+  </si>
+  <si>
+    <t>Banco BS2 S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/19173</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com › company › BONS3:BZ</t>
+  </si>
+  <si>
+    <t>Banco BTG Pactual S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18118</t>
+  </si>
+  <si>
+    <t>https://www.btgpactual.com</t>
+  </si>
+  <si>
+    <t>Banco C6 S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/19174</t>
+  </si>
+  <si>
+    <t>https://www.c6bank.com.br</t>
+  </si>
+  <si>
+    <t>BANCO DAYCOVAL S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18120</t>
+  </si>
+  <si>
+    <t>https://www.daycoval.com.br › ...</t>
+  </si>
+  <si>
+    <t>Banco do Brasil S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18123</t>
+  </si>
+  <si>
+    <t>Banco do Estado do Rio Grande do Sul S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18124</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com › profile</t>
+  </si>
+  <si>
+    <t>Banco Fibra S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18126</t>
+  </si>
+  <si>
+    <t>https://www.bancofibra.com.br</t>
+  </si>
+  <si>
+    <t>Banco General (Overseas), Inc.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18128</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu › ... › Cayman Islands</t>
+  </si>
+  <si>
+    <t>Banco Indusval S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18131</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com › company › IDVL4:BZ</t>
+  </si>
+  <si>
+    <t>Banco Mercantil del Norte, S.A., Institucion de Banca Multiple, Grupo Financiero Banorte</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18132</t>
+  </si>
+  <si>
+    <t>https://www.unepfi.org › member › banco-mercantil-de...</t>
+  </si>
+  <si>
+    <t>Banco Morgan Stanley S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18135</t>
+  </si>
+  <si>
+    <t>Banco Nacional de Comercio Exterior, SNC</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18136</t>
+  </si>
+  <si>
+    <t>Banco Original S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18674</t>
+  </si>
+  <si>
+    <t>https://www.original.com.br</t>
+  </si>
+  <si>
+    <t>Banco Pine S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18137</t>
+  </si>
+  <si>
+    <t>https://www.pine.com</t>
+  </si>
+  <si>
+    <t>Banco Safra (Cayman Islands) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18139</t>
+  </si>
+  <si>
+    <t>Banco Safra S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18140</t>
+  </si>
+  <si>
+    <t>https://www.safra.com.br</t>
+  </si>
+  <si>
+    <t>Banco Santander (Brasil) S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18141</t>
+  </si>
+  <si>
+    <t>https://www.santander.com.br › santander-brasil-en</t>
+  </si>
+  <si>
+    <t>Banco Sofisa S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18142</t>
+  </si>
+  <si>
+    <t>https://www.sofisa.com.br</t>
+  </si>
+  <si>
+    <t>Banco Sumitomo Mitsui Brasileiro S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18143</t>
+  </si>
+  <si>
+    <t>https://www.smbcgroup.com.br</t>
+  </si>
+  <si>
+    <t>Bancolombia Cayman</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18144</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18152</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18153</t>
+  </si>
+  <si>
+    <t>Barclays Bank PLC</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18157</t>
+  </si>
+  <si>
+    <t>BCP Finance Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18159</t>
+  </si>
+  <si>
+    <t>Bessemer Trust Company (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18161</t>
+  </si>
+  <si>
+    <t>https://www.bessemertrust.com › offices › grand-cayman-...</t>
+  </si>
+  <si>
+    <t>BMG Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18163</t>
+  </si>
+  <si>
+    <t>BNP Paribas Bank &amp; Trust Cayman Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18165</t>
+  </si>
+  <si>
+    <t>Brown Brothers Harriman &amp; Co.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18170</t>
+  </si>
+  <si>
+    <t>https://www.bbh.com</t>
+  </si>
+  <si>
+    <t>Butterfield Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18300</t>
+  </si>
+  <si>
+    <t>domestic and international</t>
+  </si>
+  <si>
+    <t>https://www.butterfieldgroup.com › en-ky</t>
+  </si>
+  <si>
+    <t>Cainvest Bank and Trust Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18308</t>
+  </si>
+  <si>
+    <t>https://cainvest.com</t>
+  </si>
+  <si>
+    <t>Cayman National Bank Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18302</t>
+  </si>
+  <si>
+    <t>https://www.caymannational.com</t>
+  </si>
+  <si>
+    <t>China Construction Bank (Brasil) Banco Multiplo S/A</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18130</t>
+  </si>
+  <si>
+    <t>http://www.br.ccb.com › ...</t>
+  </si>
+  <si>
+    <t>CIBC Cayman Bank Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18677</t>
+  </si>
+  <si>
+    <t>https://www.cibcfcib.com › locations › cayman-islands</t>
+  </si>
+  <si>
+    <t>CITCO Bank and Trust Company Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18177</t>
+  </si>
+  <si>
+    <t>Citizens Bank, National Association</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18250</t>
+  </si>
+  <si>
+    <t>https://www.citizensbank.com</t>
+  </si>
+  <si>
+    <t>Comerica Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18182</t>
+  </si>
+  <si>
+    <t>https://www.comerica.com</t>
+  </si>
+  <si>
+    <t>COMMERZBANK AKTIENGESELLSCHAFT</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18183</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18188</t>
+  </si>
+  <si>
+    <t>Delta Bank and Trust Company, Grand Cayman</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18189</t>
+  </si>
+  <si>
+    <t>https://cayman.directory › delta-bank-trust-grand-caym...</t>
+  </si>
+  <si>
+    <t>Deutsche Bank Aktiengesellschaft</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18190</t>
+  </si>
+  <si>
+    <t>DMS Bank &amp; Trust Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18191</t>
+  </si>
+  <si>
+    <t>https://dmsbank.com</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18192</t>
+  </si>
+  <si>
+    <t>EFG Bank AG</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18194</t>
+  </si>
+  <si>
+    <t>https://www.efgbank.com</t>
+  </si>
+  <si>
+    <t>Elant Bank &amp; Trust Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18225</t>
+  </si>
+  <si>
+    <t>Fidelity Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18305</t>
+  </si>
+  <si>
+    <t>https://www.fidelitygroup.com › caymanislands</t>
+  </si>
+  <si>
+    <t>Fifth Third Bank, National Association</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18196</t>
+  </si>
+  <si>
+    <t>https://www.53.com › fifth-third › personal-banking</t>
+  </si>
+  <si>
+    <t>FirstCaribbean International Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18306</t>
+  </si>
+  <si>
+    <t> (2.4)</t>
+  </si>
+  <si>
+    <t>FirstCaribbean International Bank and Trust Company (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18303</t>
+  </si>
+  <si>
+    <t>https://www.cibcfcib.com › private-wealth-management</t>
+  </si>
+  <si>
+    <t>Givens Hall Bank &amp; Trust Ltd</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18199</t>
+  </si>
+  <si>
+    <t>Global Fidelity Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18593</t>
+  </si>
+  <si>
+    <t>GNB Sudameris Bank Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18200</t>
+  </si>
+  <si>
+    <t>Haitong Banco de Investimento do Brasil S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18160</t>
+  </si>
+  <si>
+    <t>https://www.haitongib.com › where-we-are › sao-paulo</t>
+  </si>
+  <si>
+    <t>Heritage Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18678</t>
+  </si>
+  <si>
+    <t>https://www.heritage.com.au</t>
+  </si>
+  <si>
+    <t>Industrial and Commercial Bank of China (Asia) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18207</t>
+  </si>
+  <si>
+    <t>https://www.icbcasia.com › ICBC › 海外分行 › 工银亚洲</t>
+  </si>
+  <si>
+    <t>International Bank for Commerce</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18208</t>
+  </si>
+  <si>
+    <t>https://www.ibc.com</t>
+  </si>
+  <si>
+    <t>Itau Bank &amp; Trust Cayman Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18212</t>
+  </si>
+  <si>
+    <t>https://web.caymanchamber.ky › Banks › Itau-Bank-Tr...</t>
+  </si>
+  <si>
+    <t>Itau Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18213</t>
+  </si>
+  <si>
+    <t>https://www.itau.com</t>
+  </si>
+  <si>
+    <t>Itau Unibanco Holding S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18214</t>
+  </si>
+  <si>
+    <t>https://www.itau.com.br › relacoes-com-investidores</t>
+  </si>
+  <si>
+    <t>ITAU UNIBANCO S.A.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18215</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org › wiki › Itaú_Unibanco</t>
+  </si>
+  <si>
+    <t>Kasikornbank Public Company Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18217</t>
+  </si>
+  <si>
+    <t>https://kasikornbank.com › about › Information</t>
+  </si>
+  <si>
+    <t>Krung Thai Bank Public Company Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18220</t>
+  </si>
+  <si>
+    <t>https://krungthai.com › personal</t>
+  </si>
+  <si>
+    <t>LGT Bank (Cayman) Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18223</t>
+  </si>
+  <si>
+    <t>Manufacturers and Traders Trust Company</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18224</t>
+  </si>
+  <si>
+    <t>Merrill Lynch Bank and Trust Company (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18309</t>
+  </si>
+  <si>
+    <t>https://web.caymanchamber.ky › Trust-Companies › M...</t>
+  </si>
+  <si>
+    <t>Millennium bcp Bank &amp; Trust</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18226</t>
+  </si>
+  <si>
+    <t>https://web.caymanchamber.ky › Banks › Millennium-...</t>
+  </si>
+  <si>
+    <t>Mizuho Bank, Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18229</t>
+  </si>
+  <si>
+    <t>Morval Bank &amp; Trust Cayman Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18310</t>
+  </si>
+  <si>
+    <t>MUFG Alternative Fund Services (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18314</t>
+  </si>
+  <si>
+    <t>https://www.mufg-investorservices.com › about-us › gl...</t>
+  </si>
+  <si>
+    <t>Nacional Financiera S.N.C.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18233</t>
+  </si>
+  <si>
+    <t>https://www.nafin.com › content › h...</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18234</t>
+  </si>
+  <si>
+    <t>National Bank of Kuwait, Societe Anonyme Kuwaitienne Publique</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18236</t>
+  </si>
+  <si>
+    <t>NCB (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18238</t>
+  </si>
+  <si>
+    <t>https://ncbcaymanlimited.com</t>
+  </si>
+  <si>
+    <t>Northern Trust Company (The)</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18241</t>
+  </si>
+  <si>
+    <t>https://www.northerntrust.com › united-states</t>
+  </si>
+  <si>
+    <t>Popular Bank Llc, Cayman</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18244</t>
+  </si>
+  <si>
+    <t>PT Bank Rakyat Indonesia (Persero) TBK</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18246</t>
+  </si>
+  <si>
+    <t>https://www.ir-bri.com</t>
+  </si>
+  <si>
+    <t>PT. BANK MANDIRI (PERSERO) Tbk</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18247</t>
+  </si>
+  <si>
+    <t>https://bankmandiri.co.id</t>
+  </si>
+  <si>
+    <t>Queensgate Bank and Trust Company Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18248</t>
+  </si>
+  <si>
+    <t>https://www.queensgate.com.ky › about-us</t>
+  </si>
+  <si>
+    <t>RBC Royal Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18311</t>
+  </si>
+  <si>
+    <t> (1.7)</t>
+  </si>
+  <si>
+    <t>http://www.rbcroyalbank.com › caribbean › cayman</t>
+  </si>
+  <si>
+    <t>Regions Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18251</t>
+  </si>
+  <si>
+    <t>https://www.regions.com › personal-banking</t>
+  </si>
+  <si>
+    <t>Republic Bank (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18252</t>
+  </si>
+  <si>
+    <t>https://www.republictt.com › about › republic-bank-cay...</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18253</t>
+  </si>
+  <si>
+    <t>Scotiabank &amp; Trust (Cayman) Ltd</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18313</t>
+  </si>
+  <si>
+    <t> (2.8)</t>
+  </si>
+  <si>
+    <t>https://ky.scotiabank.com › about-scotiabank › scotiaba...</t>
+  </si>
+  <si>
+    <t>Silicon Valley Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18261</t>
+  </si>
+  <si>
+    <t>https://www.svb.com › ...</t>
+  </si>
+  <si>
+    <t>Societe Generale</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18263</t>
+  </si>
+  <si>
+    <t>St. Georges Bank &amp; Trust Company (Cayman) Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18264</t>
+  </si>
+  <si>
+    <t>https://www.stgeorgesbankcayman.com</t>
+  </si>
+  <si>
+    <t>Sumitomo Mitsui Banking Corporation</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18266</t>
+  </si>
+  <si>
+    <t>https://www.smbcgroup.com</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18274</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18275</t>
+  </si>
+  <si>
+    <t>The Siam Commercial Bank Public Company Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18280</t>
+  </si>
+  <si>
+    <t>https://www.scb.co.th › about-us</t>
+  </si>
+  <si>
+    <t>TMB Bank Public Company Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18281</t>
+  </si>
+  <si>
+    <t>https://www.tmbbank.com › ...</t>
+  </si>
+  <si>
+    <t>Toronto - Dominion Bank (The)</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18282</t>
+  </si>
+  <si>
+    <t>Towerbank, Ltd</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18283</t>
+  </si>
+  <si>
+    <t>Trade and Commerce Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18284</t>
+  </si>
+  <si>
+    <t>http://tcbliquidation.ky</t>
+  </si>
+  <si>
+    <t>Trident Trust Company (Cayman) Limited</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18285</t>
+  </si>
+  <si>
+    <t>https://tridenttrust.com › americas-and-caribbean › cay...</t>
+  </si>
+  <si>
+    <t>Truist Bank</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18168</t>
+  </si>
+  <si>
+    <t>https://www.truist.com</t>
+  </si>
+  <si>
+    <t>U.S. Bank National Association</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18286</t>
+  </si>
+  <si>
+    <t>https://www.usbank.com</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18287</t>
+  </si>
+  <si>
+    <t>United Bank for Africa Plc</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18290</t>
+  </si>
+  <si>
+    <t>https://www.ubagroup.com</t>
+  </si>
+  <si>
+    <t>VBT Bank &amp; Trust, Ltd.</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18291</t>
+  </si>
+  <si>
+    <t>https://www.vbtbank.com</t>
+  </si>
+  <si>
+    <t>Venezolano De Credito, S.A., Banco Universal</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18292</t>
+  </si>
+  <si>
+    <t>http://www.venezolano.com</t>
+  </si>
+  <si>
+    <t>Webster Bank, National Association</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18293</t>
+  </si>
+  <si>
+    <t>https://public.websteronline.com › personal</t>
+  </si>
+  <si>
+    <t>Wells Fargo Bank, National Association</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18294</t>
+  </si>
+  <si>
+    <t>https://thebanks.eu/banks/18295</t>
+  </si>
+  <si>
+    <t>URL (theBanks)</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Clients</t>
   </si>
 </sst>
 </file>
@@ -4359,10 +5254,2292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F5D2D6-A0BC-408B-9DE6-2FB98676CE28}">
+  <dimension ref="A1:F113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1616</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E1" t="s">
+        <v>843</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E4" t="s">
+        <v>854</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E39" t="s">
+        <v>925</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E41" t="s">
+        <v>906</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E50" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>296</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E53" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E56" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1473</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E61" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E63" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E64" t="s">
+        <v>49</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E65" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E66" t="s">
+        <v>49</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E67" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E68" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E70" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E71" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E72" t="s">
+        <v>49</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E73" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E74" t="s">
+        <v>49</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E75" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E76" t="s">
+        <v>49</v>
+      </c>
+      <c r="F76" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E77" t="s">
+        <v>49</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>534</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E80" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E81" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E82" t="s">
+        <v>854</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E83" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E84" t="s">
+        <v>49</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E85" t="s">
+        <v>49</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E86" t="s">
+        <v>49</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E87" t="s">
+        <v>854</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1551</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E89" t="s">
+        <v>49</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E90" t="s">
+        <v>49</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>624</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1551</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1562</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E93" t="s">
+        <v>49</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E94" t="s">
+        <v>49</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E95" t="s">
+        <v>49</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E96" t="s">
+        <v>49</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>705</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E97" t="s">
+        <v>49</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>713</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E98" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E99" t="s">
+        <v>49</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E100" t="s">
+        <v>49</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E101" t="s">
+        <v>49</v>
+      </c>
+      <c r="F101" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E102" t="s">
+        <v>49</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E103" t="s">
+        <v>49</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E104" t="s">
+        <v>49</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E105" t="s">
+        <v>49</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E106" t="s">
+        <v>49</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>766</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E107" t="s">
+        <v>49</v>
+      </c>
+      <c r="F107" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E108" t="s">
+        <v>49</v>
+      </c>
+      <c r="F108" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E109" t="s">
+        <v>49</v>
+      </c>
+      <c r="F109" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E110" t="s">
+        <v>49</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1610</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E111" t="s">
+        <v>49</v>
+      </c>
+      <c r="F111" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E112" t="s">
+        <v>49</v>
+      </c>
+      <c r="F112" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>826</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E113" t="s">
+        <v>49</v>
+      </c>
+      <c r="F113" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C0A628-0A6D-43FF-B4E0-5E18D0F86A8C}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5622,7 +8799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3D35A5-D059-4ACF-842D-672F158C38D5}">
   <dimension ref="A1:H267"/>
   <sheetViews>

</xml_diff>